<commit_message>
Nueva base de datos
</commit_message>
<xml_diff>
--- a/src/public/uploads/Poblacion.xlsx
+++ b/src/public/uploads/Poblacion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliocesarmendoza/Desktop/pipApp/Backend-pi/src/public/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85537E5-518A-EC47-90A6-353C9A3C26D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908BAECA-4C25-4B46-8DB2-3A22F2A779F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="5020" windowWidth="38400" windowHeight="19860" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1568,7 +1568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AS433"/>
   <sheetViews>
-    <sheetView topLeftCell="A391" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E458" sqref="E458"/>
     </sheetView>
   </sheetViews>
@@ -61008,8 +61008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3252A265-103C-0F4C-8DEE-5C8D1FD3E3DC}">
   <dimension ref="A1:AE22"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="Z26" sqref="Z26"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -63119,8 +63119,8 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>